<commit_message>
read and clean data portion done!!!
</commit_message>
<xml_diff>
--- a/Project/RaceProfile.xlsx
+++ b/Project/RaceProfile.xlsx
@@ -2,19 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahr\Desktop\PSTAT131\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EB3968-2BAF-4C2F-95DA-28BEC7A7F580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2620D671-76EC-4739-915F-948E48744281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,60 +47,75 @@
     <t>Distance</t>
   </si>
   <si>
+    <t>StageNum</t>
+  </si>
+  <si>
     <t>ProfileScore</t>
   </si>
   <si>
     <t>VertMeters</t>
   </si>
   <si>
+    <t>RaceRanking</t>
+  </si>
+  <si>
     <t>StartlistQualScore</t>
   </si>
   <si>
+    <t>ParcourTypeCategorical</t>
+  </si>
+  <si>
     <t>MaxAlt</t>
   </si>
   <si>
+    <t>WinningTimeHours</t>
+  </si>
+  <si>
+    <t>WinningTimeMinutes</t>
+  </si>
+  <si>
     <t>WinningTimeMin</t>
   </si>
   <si>
-    <t>StageNum</t>
+    <t>WonByCategorical</t>
+  </si>
+  <si>
+    <t>NumStarted</t>
+  </si>
+  <si>
+    <t>NumFinished</t>
+  </si>
+  <si>
+    <t>Months</t>
+  </si>
+  <si>
+    <t>Days</t>
   </si>
   <si>
     <t>PercentFinished</t>
   </si>
   <si>
-    <t>NumFinished</t>
-  </si>
-  <si>
-    <t>RaceRanking</t>
-  </si>
-  <si>
-    <t>ParcourTypeCategorical</t>
-  </si>
-  <si>
-    <t>Months</t>
-  </si>
-  <si>
-    <t>Days</t>
+    <t>DaysIntoYear</t>
   </si>
   <si>
     <t>UAEStage1</t>
   </si>
   <si>
-    <t>WinningTimeHours</t>
-  </si>
-  <si>
-    <t>WinningTimeMinutes</t>
-  </si>
-  <si>
     <t>Flat</t>
   </si>
   <si>
+    <t>Sprint</t>
+  </si>
+  <si>
     <t>UAEStage2</t>
   </si>
   <si>
     <t>UAEStage3</t>
   </si>
   <si>
+    <t>ITTFlat</t>
+  </si>
+  <si>
     <t>ITT</t>
   </si>
   <si>
@@ -109,12 +125,18 @@
     <t>MountainTop</t>
   </si>
   <si>
+    <t>GCGroup</t>
+  </si>
+  <si>
     <t>UAEStage5</t>
   </si>
   <si>
     <t>UAEStage6</t>
   </si>
   <si>
+    <t>Break</t>
+  </si>
+  <si>
     <t>UAEStage7</t>
   </si>
   <si>
@@ -124,7 +146,7 @@
     <t>CobbleHill</t>
   </si>
   <si>
-    <t>NumStarted</t>
+    <t>Solo</t>
   </si>
   <si>
     <t>Strade</t>
@@ -145,9 +167,6 @@
     <t>HillHill</t>
   </si>
   <si>
-    <t>ITTFlat</t>
-  </si>
-  <si>
     <t>ParisNiceStage4</t>
   </si>
   <si>
@@ -169,18 +188,6 @@
     <t>TirrenoStage1</t>
   </si>
   <si>
-    <t>WonByCategorical</t>
-  </si>
-  <si>
-    <t>Sprint</t>
-  </si>
-  <si>
-    <t>GCGroup</t>
-  </si>
-  <si>
-    <t>Solo</t>
-  </si>
-  <si>
     <t>TirrenoStage2</t>
   </si>
   <si>
@@ -313,9 +320,6 @@
     <t>GiroStage4</t>
   </si>
   <si>
-    <t>Break</t>
-  </si>
-  <si>
     <t>GiroStage5</t>
   </si>
   <si>
@@ -325,9 +329,6 @@
     <t>GiroStage7</t>
   </si>
   <si>
-    <t>DaysIntoYear</t>
-  </si>
-  <si>
     <t>GiroStage8</t>
   </si>
   <si>
@@ -565,10 +566,10 @@
     <t>VueltaStage21</t>
   </si>
   <si>
+    <t>Bemer</t>
+  </si>
+  <si>
     <t>Bretagne</t>
-  </si>
-  <si>
-    <t>Bemer</t>
   </si>
   <si>
     <t>Quebec</t>
@@ -630,956 +631,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$1:$R$1</c:f>
-              <c:strCache>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>RaceName</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>AvgSpeedWinner</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Distance</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>StageNum</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>ProfileScore</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>VertMeters</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>RaceRanking</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>StartlistQualScore</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>ParcourTypeCategorical</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>MaxAlt</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>WinningTimeHours</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>WinningTimeMinutes</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>WinningTimeMin</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>WonByCategorical</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>NumStarted</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>NumFinished</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Months</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Days</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$R$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>39.148936170212764</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>184</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1303</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>607</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>282</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>126</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9CDD-44D6-884F-4975E6E1C0CE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="2058307616"/>
-        <c:axId val="2058308032"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2058307616"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2058308032"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2058308032"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2058307616"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{33701FC0-2B84-4197-91AC-5B8A8505D36C}">
-  <sheetPr codeName="Chart1"/>
-  <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</chartsheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667338" cy="6292273"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{177882BB-1294-4571-BAD2-1F9194C2E995}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1845,11 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E76" workbookViewId="0">
-      <selection activeCell="Q84" sqref="Q84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1869,60 +919,60 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
       <c r="S1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <f>C2/(M2/60)</f>
@@ -1947,7 +997,7 @@
         <v>607</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J2">
         <v>201</v>
@@ -1963,7 +1013,7 @@
         <v>282</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O2">
         <v>126</v>
@@ -1988,7 +1038,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>40.499000000000002</v>
@@ -2012,7 +1062,7 @@
         <v>607</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J3">
         <v>57</v>
@@ -2028,7 +1078,7 @@
         <v>260</v>
       </c>
       <c r="N3" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O3">
         <v>125</v>
@@ -2053,7 +1103,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>55.575000000000003</v>
@@ -2077,7 +1127,7 @@
         <v>607</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J4">
         <v>4</v>
@@ -2093,7 +1143,7 @@
         <v>9</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O4">
         <v>125</v>
@@ -2118,7 +1168,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>37.526000000000003</v>
@@ -2142,7 +1192,7 @@
         <v>607</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J5">
         <v>1490</v>
@@ -2158,7 +1208,7 @@
         <v>289</v>
       </c>
       <c r="N5" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O5">
         <v>125</v>
@@ -2183,7 +1233,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>42.475999999999999</v>
@@ -2207,7 +1257,7 @@
         <v>607</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J6">
         <v>63</v>
@@ -2223,7 +1273,7 @@
         <v>257</v>
       </c>
       <c r="N6" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O6">
         <v>125</v>
@@ -2248,7 +1298,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>45.345999999999997</v>
@@ -2272,7 +1322,7 @@
         <v>607</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J7">
         <v>29</v>
@@ -2288,7 +1338,7 @@
         <v>238</v>
       </c>
       <c r="N7" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O7">
         <v>125</v>
@@ -2313,7 +1363,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>44.311</v>
@@ -2337,7 +1387,7 @@
         <v>607</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J8">
         <v>1031</v>
@@ -2353,7 +1403,7 @@
         <v>200</v>
       </c>
       <c r="N8" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O8">
         <v>125</v>
@@ -2378,7 +1428,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>41.137</v>
@@ -2402,7 +1452,7 @@
         <v>749</v>
       </c>
       <c r="I9" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="J9">
         <v>100</v>
@@ -2418,7 +1468,7 @@
         <v>290</v>
       </c>
       <c r="N9" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O9">
         <v>171</v>
@@ -2443,7 +1493,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>38.357999999999997</v>
@@ -2467,7 +1517,7 @@
         <v>662</v>
       </c>
       <c r="I10" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="J10">
         <v>324</v>
@@ -2483,7 +1533,7 @@
         <v>287</v>
       </c>
       <c r="N10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O10">
         <v>149</v>
@@ -2508,7 +1558,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>41.936</v>
@@ -2532,7 +1582,7 @@
         <v>1183</v>
       </c>
       <c r="I11" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J11">
         <v>118</v>
@@ -2548,7 +1598,7 @@
         <v>228</v>
       </c>
       <c r="N11" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O11">
         <v>154</v>
@@ -2573,7 +1623,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>47.076999999999998</v>
@@ -2597,7 +1647,7 @@
         <v>1183</v>
       </c>
       <c r="I12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J12">
         <v>174</v>
@@ -2613,7 +1663,7 @@
         <v>202</v>
       </c>
       <c r="N12" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O12">
         <v>153</v>
@@ -2638,7 +1688,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B13">
         <v>43.448999999999998</v>
@@ -2662,7 +1712,7 @@
         <v>1183</v>
       </c>
       <c r="I13" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J13">
         <v>559</v>
@@ -2678,7 +1728,7 @@
         <v>263</v>
       </c>
       <c r="N13" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O13">
         <v>149</v>
@@ -2703,7 +1753,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B14">
         <v>49.223999999999997</v>
@@ -2727,7 +1777,7 @@
         <v>1183</v>
       </c>
       <c r="I14" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J14">
         <v>299</v>
@@ -2743,7 +1793,7 @@
         <v>16</v>
       </c>
       <c r="N14" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O14">
         <v>146</v>
@@ -2768,7 +1818,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>38.595999999999997</v>
@@ -2792,7 +1842,7 @@
         <v>1183</v>
       </c>
       <c r="I15" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J15">
         <v>1201</v>
@@ -2808,7 +1858,7 @@
         <v>293</v>
       </c>
       <c r="N15" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O15">
         <v>144</v>
@@ -2833,7 +1883,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B16">
         <v>38.475000000000001</v>
@@ -2857,7 +1907,7 @@
         <v>1183</v>
       </c>
       <c r="I16" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J16">
         <v>730</v>
@@ -2873,7 +1923,7 @@
         <v>333</v>
       </c>
       <c r="N16" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O16">
         <v>121</v>
@@ -2898,7 +1948,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B17">
         <v>38.354999999999997</v>
@@ -2922,7 +1972,7 @@
         <v>1183</v>
       </c>
       <c r="I17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J17">
         <v>1605</v>
@@ -2938,7 +1988,7 @@
         <v>242</v>
       </c>
       <c r="N17" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O17">
         <v>110</v>
@@ -2963,7 +2013,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B18">
         <v>40.095999999999997</v>
@@ -2987,7 +2037,7 @@
         <v>1183</v>
       </c>
       <c r="I18" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J18">
         <v>623</v>
@@ -3003,7 +2053,7 @@
         <v>172</v>
       </c>
       <c r="N18" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O18">
         <v>96</v>
@@ -3028,7 +2078,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B19">
         <v>54.569000000000003</v>
@@ -3052,7 +2102,7 @@
         <v>1061</v>
       </c>
       <c r="I19" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -3068,7 +2118,7 @@
         <v>15</v>
       </c>
       <c r="N19" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O19">
         <v>167</v>
@@ -3093,7 +2143,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B20">
         <v>40.383000000000003</v>
@@ -3117,7 +2167,7 @@
         <v>1061</v>
       </c>
       <c r="I20" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J20">
         <v>544</v>
@@ -3133,7 +2183,7 @@
         <v>325</v>
       </c>
       <c r="N20" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O20">
         <v>167</v>
@@ -3158,7 +2208,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B21">
         <v>41.228999999999999</v>
@@ -3182,7 +2232,7 @@
         <v>1061</v>
       </c>
       <c r="I21" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J21">
         <v>552</v>
@@ -3198,7 +2248,7 @@
         <v>247</v>
       </c>
       <c r="N21" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O21">
         <v>166</v>
@@ -3223,7 +2273,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B22">
         <v>41.988999999999997</v>
@@ -3247,7 +2297,7 @@
         <v>1061</v>
       </c>
       <c r="I22" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J22">
         <v>1105</v>
@@ -3263,7 +2313,7 @@
         <v>288</v>
       </c>
       <c r="N22" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O22">
         <v>164</v>
@@ -3288,7 +2338,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B23">
         <v>42.295000000000002</v>
@@ -3312,7 +2362,7 @@
         <v>1061</v>
       </c>
       <c r="I23" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J23">
         <v>676</v>
@@ -3328,7 +2378,7 @@
         <v>219</v>
       </c>
       <c r="N23" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O23">
         <v>163</v>
@@ -3353,7 +2403,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B24">
         <v>39.216000000000001</v>
@@ -3377,7 +2427,7 @@
         <v>1061</v>
       </c>
       <c r="I24" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J24">
         <v>1366</v>
@@ -3393,7 +2443,7 @@
         <v>328</v>
       </c>
       <c r="N24" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O24">
         <v>157</v>
@@ -3418,7 +2468,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B25">
         <v>43.37</v>
@@ -3442,7 +2492,7 @@
         <v>1061</v>
       </c>
       <c r="I25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J25">
         <v>508</v>
@@ -3458,7 +2508,7 @@
         <v>219</v>
       </c>
       <c r="N25" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O25">
         <v>149</v>
@@ -3483,7 +2533,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B26">
         <v>45.331000000000003</v>
@@ -3507,7 +2557,7 @@
         <v>936</v>
       </c>
       <c r="I26" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J26">
         <v>539</v>
@@ -3523,7 +2573,7 @@
         <v>387</v>
       </c>
       <c r="N26" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O26">
         <v>166</v>
@@ -3548,7 +2598,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B27">
         <v>45.215000000000003</v>
@@ -3572,7 +2622,7 @@
         <v>722</v>
       </c>
       <c r="I27" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J27">
         <v>354</v>
@@ -3588,7 +2638,7 @@
         <v>227</v>
       </c>
       <c r="N27" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O27">
         <v>165</v>
@@ -3613,7 +2663,7 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B28">
         <v>42.69</v>
@@ -3637,7 +2687,7 @@
         <v>722</v>
       </c>
       <c r="I28" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J28">
         <v>261</v>
@@ -3653,7 +2703,7 @@
         <v>284</v>
       </c>
       <c r="N28" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O28">
         <v>164</v>
@@ -3678,7 +2728,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B29">
         <v>38.228000000000002</v>
@@ -3702,7 +2752,7 @@
         <v>772</v>
       </c>
       <c r="I29" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J29">
         <v>1788</v>
@@ -3718,7 +2768,7 @@
         <v>252</v>
       </c>
       <c r="N29" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O29">
         <v>160</v>
@@ -3743,7 +2793,7 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B30">
         <v>38.402999999999999</v>
@@ -3767,7 +2817,7 @@
         <v>772</v>
       </c>
       <c r="I30" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J30">
         <v>2049</v>
@@ -3783,7 +2833,7 @@
         <v>260</v>
       </c>
       <c r="N30" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O30">
         <v>152</v>
@@ -3808,7 +2858,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B31">
         <v>38.527000000000001</v>
@@ -3832,7 +2882,7 @@
         <v>722</v>
       </c>
       <c r="I31" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J31">
         <v>1098</v>
@@ -3848,7 +2898,7 @@
         <v>321</v>
       </c>
       <c r="N31" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O31">
         <v>143</v>
@@ -3873,7 +2923,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B32">
         <v>40.575000000000003</v>
@@ -3897,7 +2947,7 @@
         <v>722</v>
       </c>
       <c r="I32" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J32">
         <v>977</v>
@@ -3913,7 +2963,7 @@
         <v>249</v>
       </c>
       <c r="N32" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O32">
         <v>140</v>
@@ -3938,7 +2988,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B33">
         <v>41.968000000000004</v>
@@ -3962,7 +3012,7 @@
         <v>722</v>
       </c>
       <c r="I33" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J33">
         <v>425</v>
@@ -3978,7 +3028,7 @@
         <v>198</v>
       </c>
       <c r="N33" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O33">
         <v>114</v>
@@ -4003,7 +3053,7 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B34">
         <v>43.664000000000001</v>
@@ -4027,7 +3077,7 @@
         <v>459</v>
       </c>
       <c r="I34" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J34">
         <v>14</v>
@@ -4043,7 +3093,7 @@
         <v>285</v>
       </c>
       <c r="N34" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O34">
         <v>164</v>
@@ -4068,7 +3118,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B35">
         <v>43.997</v>
@@ -4092,7 +3142,7 @@
         <v>636</v>
       </c>
       <c r="I35" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="J35">
         <v>150</v>
@@ -4108,7 +3158,7 @@
         <v>278</v>
       </c>
       <c r="N35" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O35">
         <v>175</v>
@@ -4133,7 +3183,7 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B36">
         <v>44.171999999999997</v>
@@ -4157,7 +3207,7 @@
         <v>838</v>
       </c>
       <c r="I36" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J36">
         <v>154</v>
@@ -4173,7 +3223,7 @@
         <v>337</v>
       </c>
       <c r="N36" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O36">
         <v>174</v>
@@ -4198,7 +3248,7 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B37">
         <v>44.869</v>
@@ -4222,7 +3272,7 @@
         <v>647</v>
       </c>
       <c r="I37" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J37">
         <v>153</v>
@@ -4238,7 +3288,7 @@
         <v>245</v>
       </c>
       <c r="N37" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O37">
         <v>171</v>
@@ -4263,7 +3313,7 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B38">
         <v>43.197000000000003</v>
@@ -4287,7 +3337,7 @@
         <v>759</v>
       </c>
       <c r="I38" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="J38">
         <v>150</v>
@@ -4303,7 +3353,7 @@
         <v>378</v>
       </c>
       <c r="N38" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O38">
         <v>167</v>
@@ -4328,7 +3378,7 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B39">
         <v>45.98</v>
@@ -4352,7 +3402,7 @@
         <v>742</v>
       </c>
       <c r="I39" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J39">
         <v>60</v>
@@ -4368,7 +3418,7 @@
         <v>9</v>
       </c>
       <c r="N39" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O39">
         <v>156</v>
@@ -4393,7 +3443,7 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B40">
         <v>40.96</v>
@@ -4417,7 +3467,7 @@
         <v>742</v>
       </c>
       <c r="I40" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J40">
         <v>1052</v>
@@ -4433,7 +3483,7 @@
         <v>304</v>
       </c>
       <c r="N40" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O40">
         <v>155</v>
@@ -4458,7 +3508,7 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B41">
         <v>39.585999999999999</v>
@@ -4482,7 +3532,7 @@
         <v>742</v>
       </c>
       <c r="I41" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J41">
         <v>719</v>
@@ -4498,7 +3548,7 @@
         <v>275</v>
       </c>
       <c r="N41" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O41">
         <v>151</v>
@@ -4523,7 +3573,7 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B42">
         <v>43.604999999999997</v>
@@ -4547,7 +3597,7 @@
         <v>742</v>
       </c>
       <c r="I42" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J42">
         <v>412</v>
@@ -4563,7 +3613,7 @@
         <v>255</v>
       </c>
       <c r="N42" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O42">
         <v>142</v>
@@ -4588,7 +3638,7 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B43">
         <v>39.765000000000001</v>
@@ -4612,7 +3662,7 @@
         <v>742</v>
       </c>
       <c r="I43" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J43">
         <v>556</v>
@@ -4628,7 +3678,7 @@
         <v>247</v>
       </c>
       <c r="N43" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O43">
         <v>139</v>
@@ -4653,7 +3703,7 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B44">
         <v>35.848999999999997</v>
@@ -4677,7 +3727,7 @@
         <v>742</v>
       </c>
       <c r="I44" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J44">
         <v>678</v>
@@ -4693,7 +3743,7 @@
         <v>227</v>
       </c>
       <c r="N44" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O44">
         <v>120</v>
@@ -4718,7 +3768,7 @@
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B45">
         <v>42.195999999999998</v>
@@ -4742,7 +3792,7 @@
         <v>702</v>
       </c>
       <c r="I45" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J45">
         <v>271</v>
@@ -4758,7 +3808,7 @@
         <v>361</v>
       </c>
       <c r="N45" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O45">
         <v>170</v>
@@ -4783,7 +3833,7 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B46">
         <v>45.792000000000002</v>
@@ -4807,7 +3857,7 @@
         <v>752</v>
       </c>
       <c r="I46" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J46">
         <v>138</v>
@@ -4823,7 +3873,7 @@
         <v>337</v>
       </c>
       <c r="N46" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O46">
         <v>170</v>
@@ -4848,7 +3898,7 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B47">
         <v>42.97</v>
@@ -4872,7 +3922,7 @@
         <v>974</v>
       </c>
       <c r="I47" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J47">
         <v>297</v>
@@ -4888,7 +3938,7 @@
         <v>282</v>
       </c>
       <c r="N47" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O47">
         <v>175</v>
@@ -4913,7 +3963,7 @@
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B48">
         <v>41.412999999999997</v>
@@ -4937,7 +3987,7 @@
         <v>1101</v>
       </c>
       <c r="I48" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J48">
         <v>562</v>
@@ -4953,7 +4003,7 @@
         <v>372</v>
       </c>
       <c r="N48" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O48">
         <v>175</v>
@@ -4978,7 +4028,7 @@
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B49">
         <v>52.363999999999997</v>
@@ -5002,7 +4052,7 @@
         <v>506</v>
       </c>
       <c r="I49" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J49">
         <v>607</v>
@@ -5018,7 +4068,7 @@
         <v>5</v>
       </c>
       <c r="N49" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O49">
         <v>137</v>
@@ -5043,7 +4093,7 @@
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B50">
         <v>40.46</v>
@@ -5067,7 +4117,7 @@
         <v>506</v>
       </c>
       <c r="I50" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J50">
         <v>803</v>
@@ -5083,7 +4133,7 @@
         <v>263</v>
       </c>
       <c r="N50" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O50">
         <v>137</v>
@@ -5108,7 +4158,7 @@
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B51">
         <v>41.206000000000003</v>
@@ -5132,7 +4182,7 @@
         <v>506</v>
       </c>
       <c r="I51" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J51">
         <v>867</v>
@@ -5148,7 +4198,7 @@
         <v>244</v>
       </c>
       <c r="N51" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O51">
         <v>135</v>
@@ -5173,7 +4223,7 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B52">
         <v>42.433</v>
@@ -5197,7 +4247,7 @@
         <v>506</v>
       </c>
       <c r="I52" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J52">
         <v>759</v>
@@ -5213,7 +4263,7 @@
         <v>233</v>
       </c>
       <c r="N52" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O52">
         <v>132</v>
@@ -5238,7 +4288,7 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B53">
         <v>36.156999999999996</v>
@@ -5262,7 +4312,7 @@
         <v>506</v>
       </c>
       <c r="I53" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J53">
         <v>1664</v>
@@ -5278,7 +4328,7 @@
         <v>298</v>
       </c>
       <c r="N53" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O53">
         <v>131</v>
@@ -5303,7 +4353,7 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B54">
         <v>28.23</v>
@@ -5327,7 +4377,7 @@
         <v>506</v>
       </c>
       <c r="I54" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J54">
         <v>1256</v>
@@ -5343,7 +4393,7 @@
         <v>33</v>
       </c>
       <c r="N54" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O54">
         <v>118</v>
@@ -5368,7 +4418,7 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B55">
         <v>41.439</v>
@@ -5392,7 +4442,7 @@
         <v>309</v>
       </c>
       <c r="I55" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J55">
         <v>841</v>
@@ -5408,7 +4458,7 @@
         <v>267</v>
       </c>
       <c r="N55" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O55">
         <v>131</v>
@@ -5433,7 +4483,7 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B56">
         <v>42.472999999999999</v>
@@ -5457,7 +4507,7 @@
         <v>816</v>
       </c>
       <c r="I56" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J56">
         <v>337</v>
@@ -5473,7 +4523,7 @@
         <v>275</v>
       </c>
       <c r="N56" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O56">
         <v>176</v>
@@ -5498,7 +4548,7 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B57">
         <v>46.648000000000003</v>
@@ -5522,7 +4572,7 @@
         <v>816</v>
       </c>
       <c r="I57" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J57">
         <v>166</v>
@@ -5538,7 +4588,7 @@
         <v>11</v>
       </c>
       <c r="N57" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O57">
         <v>176</v>
@@ -5563,7 +4613,7 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B58">
         <v>40.654000000000003</v>
@@ -5587,7 +4637,7 @@
         <v>816</v>
       </c>
       <c r="I58" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J58">
         <v>189</v>
@@ -5603,7 +4653,7 @@
         <v>296</v>
       </c>
       <c r="N58" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O58">
         <v>176</v>
@@ -5628,7 +4678,7 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B59">
         <v>37.915999999999997</v>
@@ -5652,7 +4702,7 @@
         <v>816</v>
       </c>
       <c r="I59" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J59">
         <v>1899</v>
@@ -5668,7 +4718,7 @@
         <v>272</v>
       </c>
       <c r="N59" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O59">
         <v>175</v>
@@ -5693,7 +4743,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B60">
         <v>42.798999999999999</v>
@@ -5717,7 +4767,7 @@
         <v>816</v>
       </c>
       <c r="I60" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J60">
         <v>1113</v>
@@ -5733,7 +4783,7 @@
         <v>243</v>
       </c>
       <c r="N60" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O60">
         <v>173</v>
@@ -5758,7 +4808,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B61">
         <v>38.076000000000001</v>
@@ -5782,7 +4832,7 @@
         <v>816</v>
       </c>
       <c r="I61" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J61">
         <v>515</v>
@@ -5798,7 +4848,7 @@
         <v>302</v>
       </c>
       <c r="N61" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O61">
         <v>172</v>
@@ -5823,7 +4873,7 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B62">
         <v>37.631999999999998</v>
@@ -5847,7 +4897,7 @@
         <v>816</v>
       </c>
       <c r="I62" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J62">
         <v>1410</v>
@@ -5863,7 +4913,7 @@
         <v>312</v>
       </c>
       <c r="N62" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O62">
         <v>172</v>
@@ -5912,7 +4962,7 @@
         <v>816</v>
       </c>
       <c r="I63" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J63">
         <v>157</v>
@@ -5928,7 +4978,7 @@
         <v>212</v>
       </c>
       <c r="N63" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O63">
         <v>168</v>
@@ -5977,7 +5027,7 @@
         <v>816</v>
       </c>
       <c r="I64" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J64">
         <v>1664</v>
@@ -5993,7 +5043,7 @@
         <v>334</v>
       </c>
       <c r="N64" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O64">
         <v>167</v>
@@ -6042,7 +5092,7 @@
         <v>816</v>
       </c>
       <c r="I65" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J65">
         <v>281</v>
@@ -6058,7 +5108,7 @@
         <v>272</v>
       </c>
       <c r="N65" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O65">
         <v>166</v>
@@ -6107,7 +5157,7 @@
         <v>816</v>
       </c>
       <c r="I66" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J66">
         <v>67</v>
@@ -6123,7 +5173,7 @@
         <v>259</v>
       </c>
       <c r="N66" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O66">
         <v>166</v>
@@ -6172,7 +5222,7 @@
         <v>816</v>
       </c>
       <c r="I67" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J67">
         <v>957</v>
@@ -6188,7 +5238,7 @@
         <v>266</v>
       </c>
       <c r="N67" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O67">
         <v>165</v>
@@ -6237,7 +5287,7 @@
         <v>816</v>
       </c>
       <c r="I68" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J68">
         <v>938</v>
@@ -6253,7 +5303,7 @@
         <v>198</v>
       </c>
       <c r="N68" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O68">
         <v>164</v>
@@ -6302,7 +5352,7 @@
         <v>816</v>
       </c>
       <c r="I69" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J69">
         <v>688</v>
@@ -6318,7 +5368,7 @@
         <v>223</v>
       </c>
       <c r="N69" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O69">
         <v>163</v>
@@ -6367,7 +5417,7 @@
         <v>816</v>
       </c>
       <c r="I70" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J70">
         <v>1622</v>
@@ -6383,7 +5433,7 @@
         <v>277</v>
       </c>
       <c r="N70" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O70">
         <v>159</v>
@@ -6432,7 +5482,7 @@
         <v>816</v>
       </c>
       <c r="I71" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J71">
         <v>1929</v>
@@ -6448,7 +5498,7 @@
         <v>340</v>
       </c>
       <c r="N71" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O71">
         <v>158</v>
@@ -6497,7 +5547,7 @@
         <v>816</v>
       </c>
       <c r="I72" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J72">
         <v>1876</v>
@@ -6513,7 +5563,7 @@
         <v>267</v>
       </c>
       <c r="N72" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O72">
         <v>155</v>
@@ -6562,7 +5612,7 @@
         <v>816</v>
       </c>
       <c r="I73" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J73">
         <v>347</v>
@@ -6578,7 +5628,7 @@
         <v>201</v>
       </c>
       <c r="N73" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O73">
         <v>153</v>
@@ -6627,7 +5677,7 @@
         <v>816</v>
       </c>
       <c r="I74" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J74">
         <v>1136</v>
@@ -6643,7 +5693,7 @@
         <v>272</v>
       </c>
       <c r="N74" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O74">
         <v>152</v>
@@ -6692,7 +5742,7 @@
         <v>816</v>
       </c>
       <c r="I75" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J75">
         <v>2236</v>
@@ -6708,7 +5758,7 @@
         <v>286</v>
       </c>
       <c r="N75" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O75">
         <v>150</v>
@@ -6757,7 +5807,7 @@
         <v>816</v>
       </c>
       <c r="I76" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J76">
         <v>298</v>
@@ -6773,7 +5823,7 @@
         <v>22</v>
       </c>
       <c r="N76" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O76">
         <v>149</v>
@@ -6822,7 +5872,7 @@
         <v>788</v>
       </c>
       <c r="I77" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J77">
         <v>785</v>
@@ -6838,7 +5888,7 @@
         <v>277</v>
       </c>
       <c r="N77" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O77">
         <v>154</v>
@@ -6887,7 +5937,7 @@
         <v>788</v>
       </c>
       <c r="I78" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J78">
         <v>1315</v>
@@ -6903,7 +5953,7 @@
         <v>243</v>
       </c>
       <c r="N78" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O78">
         <v>151</v>
@@ -6952,7 +6002,7 @@
         <v>788</v>
       </c>
       <c r="I79" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J79">
         <v>1391</v>
@@ -6968,7 +6018,7 @@
         <v>249</v>
       </c>
       <c r="N79" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O79">
         <v>148</v>
@@ -7017,7 +6067,7 @@
         <v>788</v>
       </c>
       <c r="I80" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J80">
         <v>406</v>
@@ -7033,7 +6083,7 @@
         <v>35</v>
       </c>
       <c r="N80" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O80">
         <v>148</v>
@@ -7082,7 +6132,7 @@
         <v>788</v>
       </c>
       <c r="I81" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J81">
         <v>824</v>
@@ -7098,7 +6148,7 @@
         <v>218</v>
       </c>
       <c r="N81" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O81">
         <v>148</v>
@@ -7147,7 +6197,7 @@
         <v>788</v>
       </c>
       <c r="I82" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J82">
         <v>1241</v>
@@ -7163,7 +6213,7 @@
         <v>262</v>
       </c>
       <c r="N82" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O82">
         <v>147</v>
@@ -7212,7 +6262,7 @@
         <v>788</v>
       </c>
       <c r="I83" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J83">
         <v>2620</v>
@@ -7228,7 +6278,7 @@
         <v>233</v>
       </c>
       <c r="N83" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O83">
         <v>141</v>
@@ -7277,7 +6327,7 @@
         <v>788</v>
       </c>
       <c r="I84" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J84">
         <v>1607</v>
@@ -7293,7 +6343,7 @@
         <v>229</v>
       </c>
       <c r="N84" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O84">
         <v>135</v>
@@ -7342,7 +6392,7 @@
         <v>767</v>
       </c>
       <c r="I85" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J85">
         <v>680</v>
@@ -7358,7 +6408,7 @@
         <v>256</v>
       </c>
       <c r="N85" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O85">
         <v>153</v>
@@ -7407,7 +6457,7 @@
         <v>767</v>
       </c>
       <c r="I86" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J86">
         <v>745</v>
@@ -7423,7 +6473,7 @@
         <v>286</v>
       </c>
       <c r="N86" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O86">
         <v>152</v>
@@ -7472,7 +6522,7 @@
         <v>767</v>
       </c>
       <c r="I87" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J87">
         <v>936</v>
@@ -7488,7 +6538,7 @@
         <v>268</v>
       </c>
       <c r="N87" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O87">
         <v>150</v>
@@ -7537,7 +6587,7 @@
         <v>767</v>
       </c>
       <c r="I88" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J88">
         <v>785</v>
@@ -7553,7 +6603,7 @@
         <v>254</v>
       </c>
       <c r="N88" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O88">
         <v>148</v>
@@ -7602,7 +6652,7 @@
         <v>767</v>
       </c>
       <c r="I89" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J89">
         <v>990</v>
@@ -7618,7 +6668,7 @@
         <v>270</v>
       </c>
       <c r="N89" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O89">
         <v>143</v>
@@ -7667,7 +6717,7 @@
         <v>767</v>
       </c>
       <c r="I90" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J90">
         <v>2478</v>
@@ -7683,7 +6733,7 @@
         <v>311</v>
       </c>
       <c r="N90" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O90">
         <v>123</v>
@@ -7732,7 +6782,7 @@
         <v>767</v>
       </c>
       <c r="I91" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J91">
         <v>1976</v>
@@ -7748,7 +6798,7 @@
         <v>306</v>
       </c>
       <c r="N91" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O91">
         <v>87</v>
@@ -7797,7 +6847,7 @@
         <v>767</v>
       </c>
       <c r="I92" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J92">
         <v>457</v>
@@ -7813,7 +6863,7 @@
         <v>28</v>
       </c>
       <c r="N92" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O92">
         <v>81</v>
@@ -7862,7 +6912,7 @@
         <v>1550</v>
       </c>
       <c r="I93" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J93">
         <v>8</v>
@@ -7878,7 +6928,7 @@
         <v>15</v>
       </c>
       <c r="N93" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O93">
         <v>175</v>
@@ -7927,7 +6977,7 @@
         <v>1550</v>
       </c>
       <c r="I94" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J94">
         <v>77</v>
@@ -7943,7 +6993,7 @@
         <v>274</v>
       </c>
       <c r="N94" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O94">
         <v>175</v>
@@ -7992,7 +7042,7 @@
         <v>1550</v>
       </c>
       <c r="I95" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J95">
         <v>109</v>
@@ -8008,7 +7058,7 @@
         <v>251</v>
       </c>
       <c r="N95" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O95">
         <v>175</v>
@@ -8057,7 +7107,7 @@
         <v>1550</v>
       </c>
       <c r="I96" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J96">
         <v>204</v>
@@ -8073,7 +7123,7 @@
         <v>241</v>
       </c>
       <c r="N96" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O96">
         <v>175</v>
@@ -8122,7 +7172,7 @@
         <v>1550</v>
       </c>
       <c r="I97" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J97">
         <v>76</v>
@@ -8138,7 +7188,7 @@
         <v>193</v>
       </c>
       <c r="N97" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O97">
         <v>175</v>
@@ -8187,7 +7237,7 @@
         <v>1550</v>
       </c>
       <c r="I98" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J98">
         <v>383</v>
@@ -8203,7 +7253,7 @@
         <v>267</v>
       </c>
       <c r="N98" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O98">
         <v>173</v>
@@ -8252,7 +7302,7 @@
         <v>1550</v>
       </c>
       <c r="I99" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J99">
         <v>1141</v>
@@ -8268,7 +7318,7 @@
         <v>238</v>
       </c>
       <c r="N99" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O99">
         <v>171</v>
@@ -8317,7 +7367,7 @@
         <v>1550</v>
       </c>
       <c r="I100" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J100">
         <v>1178</v>
@@ -8333,7 +7383,7 @@
         <v>253</v>
       </c>
       <c r="N100" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O100">
         <v>171</v>
@@ -8382,7 +7432,7 @@
         <v>1550</v>
       </c>
       <c r="I101" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J101">
         <v>1769</v>
@@ -8398,7 +7448,7 @@
         <v>286</v>
       </c>
       <c r="N101" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O101">
         <v>167</v>
@@ -8447,7 +7497,7 @@
         <v>1550</v>
       </c>
       <c r="I102" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J102">
         <v>1435</v>
@@ -8463,7 +7513,7 @@
         <v>198</v>
       </c>
       <c r="N102" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O102">
         <v>164</v>
@@ -8512,7 +7562,7 @@
         <v>1550</v>
       </c>
       <c r="I103" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J103">
         <v>2630</v>
@@ -8528,7 +7578,7 @@
         <v>258</v>
       </c>
       <c r="N103" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O103">
         <v>160</v>
@@ -8577,7 +7627,7 @@
         <v>1550</v>
       </c>
       <c r="I104" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J104">
         <v>2619</v>
@@ -8593,7 +7643,7 @@
         <v>295</v>
       </c>
       <c r="N104" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O104">
         <v>158</v>
@@ -8642,7 +7692,7 @@
         <v>1550</v>
       </c>
       <c r="I105" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J105">
         <v>718</v>
@@ -8658,7 +7708,7 @@
         <v>253</v>
       </c>
       <c r="N105" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O105">
         <v>158</v>
@@ -8707,7 +7757,7 @@
         <v>1550</v>
       </c>
       <c r="I106" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J106">
         <v>1431</v>
@@ -8723,7 +7773,7 @@
         <v>270</v>
       </c>
       <c r="N106" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O106">
         <v>156</v>
@@ -8772,7 +7822,7 @@
         <v>1550</v>
       </c>
       <c r="I107" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J107">
         <v>695</v>
@@ -8788,7 +7838,7 @@
         <v>267</v>
       </c>
       <c r="N107" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O107">
         <v>156</v>
@@ -8837,7 +7887,7 @@
         <v>1550</v>
       </c>
       <c r="I108" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J108">
         <v>1511</v>
@@ -8853,7 +7903,7 @@
         <v>263</v>
       </c>
       <c r="N108" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O108">
         <v>151</v>
@@ -8902,7 +7952,7 @@
         <v>1550</v>
       </c>
       <c r="I109" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J109">
         <v>1566</v>
@@ -8918,7 +7968,7 @@
         <v>205</v>
       </c>
       <c r="N109" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O109">
         <v>145</v>
@@ -8967,7 +8017,7 @@
         <v>1550</v>
       </c>
       <c r="I110" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J110">
         <v>1703</v>
@@ -8983,7 +8033,7 @@
         <v>239</v>
       </c>
       <c r="N110" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O110">
         <v>142</v>
@@ -9032,7 +8082,7 @@
         <v>1550</v>
       </c>
       <c r="I111" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J111">
         <v>305</v>
@@ -9048,7 +8098,7 @@
         <v>232</v>
       </c>
       <c r="N111" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O111">
         <v>139</v>
@@ -9097,7 +8147,7 @@
         <v>1550</v>
       </c>
       <c r="I112" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J112">
         <v>389</v>
@@ -9113,7 +8163,7 @@
         <v>47</v>
       </c>
       <c r="N112" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O112">
         <v>138</v>
@@ -9162,7 +8212,7 @@
         <v>1550</v>
       </c>
       <c r="I113" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J113">
         <v>173</v>
@@ -9178,7 +8228,7 @@
         <v>178</v>
       </c>
       <c r="N113" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O113">
         <v>137</v>
@@ -9227,7 +8277,7 @@
         <v>724</v>
       </c>
       <c r="I114" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J114">
         <v>675</v>
@@ -9243,7 +8293,7 @@
         <v>331</v>
       </c>
       <c r="N114" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O114">
         <v>156</v>
@@ -9292,7 +8342,7 @@
         <v>467</v>
       </c>
       <c r="I115" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J115">
         <v>285</v>
@@ -9308,7 +8358,7 @@
         <v>318</v>
       </c>
       <c r="N115" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O115">
         <v>160</v>
@@ -9357,7 +8407,7 @@
         <v>467</v>
       </c>
       <c r="I116" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J116">
         <v>270</v>
@@ -9373,7 +8423,7 @@
         <v>287</v>
       </c>
       <c r="N116" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O116">
         <v>159</v>
@@ -9422,7 +8472,7 @@
         <v>467</v>
       </c>
       <c r="I117" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J117">
         <v>444</v>
@@ -9438,7 +8488,7 @@
         <v>325</v>
       </c>
       <c r="N117" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O117">
         <v>150</v>
@@ -9487,7 +8537,7 @@
         <v>467</v>
       </c>
       <c r="I118" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J118">
         <v>700</v>
@@ -9503,7 +8553,7 @@
         <v>261</v>
       </c>
       <c r="N118" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O118">
         <v>150</v>
@@ -9552,7 +8602,7 @@
         <v>467</v>
       </c>
       <c r="I119" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J119">
         <v>395</v>
@@ -9568,7 +8618,7 @@
         <v>256</v>
       </c>
       <c r="N119" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O119">
         <v>140</v>
@@ -9617,7 +8667,7 @@
         <v>467</v>
       </c>
       <c r="I120" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J120">
         <v>963</v>
@@ -9633,7 +8683,7 @@
         <v>17</v>
       </c>
       <c r="N120" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O120">
         <v>137</v>
@@ -9682,7 +8732,7 @@
         <v>467</v>
       </c>
       <c r="I121" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J121">
         <v>597</v>
@@ -9698,7 +8748,7 @@
         <v>239</v>
       </c>
       <c r="N121" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O121">
         <v>128</v>
@@ -9747,7 +8797,7 @@
         <v>970</v>
       </c>
       <c r="I122" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J122">
         <v>71</v>
@@ -9763,7 +8813,7 @@
         <v>229</v>
       </c>
       <c r="N122" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O122">
         <v>182</v>
@@ -9812,7 +8862,7 @@
         <v>970</v>
       </c>
       <c r="I123" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J123">
         <v>29</v>
@@ -9828,7 +8878,7 @@
         <v>245</v>
       </c>
       <c r="N123" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O123">
         <v>181</v>
@@ -9877,7 +8927,7 @@
         <v>970</v>
       </c>
       <c r="I124" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J124">
         <v>1094</v>
@@ -9893,7 +8943,7 @@
         <v>211</v>
       </c>
       <c r="N124" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O124">
         <v>180</v>
@@ -9942,7 +8992,7 @@
         <v>970</v>
       </c>
       <c r="I125" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J125">
         <v>428</v>
@@ -9958,7 +9008,7 @@
         <v>255</v>
       </c>
       <c r="N125" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O125">
         <v>180</v>
@@ -10007,7 +9057,7 @@
         <v>970</v>
       </c>
       <c r="I126" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J126">
         <v>1131</v>
@@ -10023,7 +9073,7 @@
         <v>278</v>
       </c>
       <c r="N126" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O126">
         <v>179</v>
@@ -10072,7 +9122,7 @@
         <v>970</v>
       </c>
       <c r="I127" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J127">
         <v>1599</v>
@@ -10088,7 +9138,7 @@
         <v>270</v>
       </c>
       <c r="N127" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O127">
         <v>178</v>
@@ -10137,7 +9187,7 @@
         <v>970</v>
       </c>
       <c r="I128" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J128">
         <v>1084</v>
@@ -10153,7 +9203,7 @@
         <v>245</v>
       </c>
       <c r="N128" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O128">
         <v>175</v>
@@ -10202,7 +9252,7 @@
         <v>970</v>
       </c>
       <c r="I129" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J129">
         <v>743</v>
@@ -10218,7 +9268,7 @@
         <v>272</v>
       </c>
       <c r="N129" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O129">
         <v>169</v>
@@ -10267,7 +9317,7 @@
         <v>970</v>
       </c>
       <c r="I130" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J130">
         <v>79</v>
@@ -10283,7 +9333,7 @@
         <v>33</v>
       </c>
       <c r="N130" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O130">
         <v>164</v>
@@ -10332,7 +9382,7 @@
         <v>970</v>
       </c>
       <c r="I131" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J131">
         <v>331</v>
@@ -10348,7 +9398,7 @@
         <v>303</v>
       </c>
       <c r="N131" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O131">
         <v>156</v>
@@ -10397,7 +9447,7 @@
         <v>970</v>
       </c>
       <c r="I132" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J132">
         <v>1260</v>
@@ -10413,7 +9463,7 @@
         <v>278</v>
       </c>
       <c r="N132" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O132">
         <v>150</v>
@@ -10462,7 +9512,7 @@
         <v>970</v>
       </c>
       <c r="I133" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J133">
         <v>765</v>
@@ -10478,7 +9528,7 @@
         <v>226</v>
       </c>
       <c r="N133" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O133">
         <v>147</v>
@@ -10527,7 +9577,7 @@
         <v>970</v>
       </c>
       <c r="I134" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J134">
         <v>1815</v>
@@ -10543,7 +9593,7 @@
         <v>249</v>
       </c>
       <c r="N134" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O134">
         <v>146</v>
@@ -10592,7 +9642,7 @@
         <v>970</v>
       </c>
       <c r="I135" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J135">
         <v>2507</v>
@@ -10608,7 +9658,7 @@
         <v>257</v>
       </c>
       <c r="N135" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O135">
         <v>145</v>
@@ -10657,7 +9707,7 @@
         <v>970</v>
       </c>
       <c r="I136" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J136">
         <v>133</v>
@@ -10673,7 +9723,7 @@
         <v>285</v>
       </c>
       <c r="N136" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O136">
         <v>144</v>
@@ -10722,7 +9772,7 @@
         <v>970</v>
       </c>
       <c r="I137" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J137">
         <v>1095</v>
@@ -10738,7 +9788,7 @@
         <v>222</v>
       </c>
       <c r="N137" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O137">
         <v>142</v>
@@ -10787,7 +9837,7 @@
         <v>970</v>
       </c>
       <c r="I138" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J138">
         <v>1269</v>
@@ -10803,7 +9853,7 @@
         <v>285</v>
       </c>
       <c r="N138" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O138">
         <v>138</v>
@@ -10852,7 +9902,7 @@
         <v>970</v>
       </c>
       <c r="I139" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J139">
         <v>1223</v>
@@ -10868,7 +9918,7 @@
         <v>199</v>
       </c>
       <c r="N139" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O139">
         <v>134</v>
@@ -10917,7 +9967,7 @@
         <v>970</v>
       </c>
       <c r="I140" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J140">
         <v>1853</v>
@@ -10933,7 +9983,7 @@
         <v>281</v>
       </c>
       <c r="N140" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O140">
         <v>134</v>
@@ -10982,7 +10032,7 @@
         <v>970</v>
       </c>
       <c r="I141" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J141">
         <v>754</v>
@@ -10998,7 +10048,7 @@
         <v>146</v>
       </c>
       <c r="N141" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="O141">
         <v>134</v>
@@ -11023,7 +10073,7 @@
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B142">
         <v>44.277999999999999</v>
@@ -11047,7 +10097,7 @@
         <v>651</v>
       </c>
       <c r="I142" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J142">
         <v>74</v>
@@ -11063,7 +10113,7 @@
         <v>277</v>
       </c>
       <c r="N142" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O142">
         <v>147</v>
@@ -11088,7 +10138,7 @@
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B143">
         <v>41.957999999999998</v>
@@ -11112,7 +10162,7 @@
         <v>812</v>
       </c>
       <c r="I143" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J143">
         <v>241</v>
@@ -11128,7 +10178,7 @@
         <v>364</v>
       </c>
       <c r="N143" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O143">
         <v>166</v>
@@ -11177,7 +10227,7 @@
         <v>866</v>
       </c>
       <c r="I144" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J144">
         <v>92</v>
@@ -11193,7 +10243,7 @@
         <v>286</v>
       </c>
       <c r="N144" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O144">
         <v>147</v>
@@ -11242,7 +10292,7 @@
         <v>864</v>
       </c>
       <c r="I145" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J145">
         <v>208</v>
@@ -11258,7 +10308,7 @@
         <v>359</v>
       </c>
       <c r="N145" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O145">
         <v>145</v>
@@ -11307,7 +10357,7 @@
         <v>1019</v>
       </c>
       <c r="I146" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J146">
         <v>1061</v>
@@ -11323,7 +10373,7 @@
         <v>381</v>
       </c>
       <c r="N146" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O146">
         <v>175</v>

</xml_diff>